<commit_message>
Add Kemetic Wonder Temple of Thoth
AB4-327
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,6 +2189,9 @@
       <c r="M15">
         <v>5</v>
       </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Add Add Kemetic Wonder Temple of Ptah
Also updated techs for other kemetic wonders

AB4-325
AB5-326
AB4-328
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -526,6 +526,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,7 +554,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,48 +844,48 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="37" t="s">
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="34" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37" t="s">
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="34" t="s">
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37" t="s">
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="40"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,7 +1970,7 @@
       <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="31" t="s">
         <v>33</v>
       </c>
       <c r="M6" t="s">
@@ -2190,7 +2190,22 @@
         <v>5</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Zoroastrian Wonder (Hammurabi Stele of Laws)
AB4-337
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,16 +2259,16 @@
         <v>3</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R18">
         <v>2</v>
@@ -2277,7 +2277,7 @@
         <v>1</v>
       </c>
       <c r="T18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Jewish wonder Masada
AB4-338
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,6 +2166,24 @@
       <c r="M14">
         <v>2</v>
       </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Add Asatru wonder Freya Sanctuary
AB4-350
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,7 +2021,22 @@
         <v>34</v>
       </c>
       <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
         <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2089,16 +2104,16 @@
         <v>4</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q11">
         <v>4</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -2277,16 +2292,16 @@
         <v>3</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P18">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="Q18">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R18">
         <v>2</v>
@@ -2295,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="T18">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Asatru wonder Thor Sanctuary
AB4-352
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,19 +2024,19 @@
         <v>3</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P7">
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <v>7</v>
+      </c>
+      <c r="T7">
         <v>4</v>
-      </c>
-      <c r="Q7">
-        <v>3</v>
-      </c>
-      <c r="T7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Confucian Wonder San Kong
AB4-365
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,6 +2089,21 @@
       <c r="M10">
         <v>2</v>
       </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Add Buddhist wonder Kotoku-in
AB4-368
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1923,7 +1923,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,6 +2052,24 @@
       <c r="M8">
         <v>4</v>
       </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
Add Buddhist wonder Nara Giant Buddha
AB4-370
</commit_message>
<xml_diff>
--- a/Support/Docs/GeneralValues.xlsx
+++ b/Support/Docs/GeneralValues.xlsx
@@ -1922,7 +1922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
@@ -2053,22 +2053,25 @@
         <v>4</v>
       </c>
       <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8">
+        <v>11</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
         <v>2</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>7</v>
-      </c>
-      <c r="Q8">
-        <v>6</v>
-      </c>
-      <c r="R8">
-        <v>2</v>
-      </c>
       <c r="T8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>